<commit_message>
data fields converted to string
</commit_message>
<xml_diff>
--- a/accepted_candidates.xlsx
+++ b/accepted_candidates.xlsx
@@ -370,16 +370,16 @@
         <v>303</v>
       </c>
       <c r="C3" t="str">
-        <v>abc</v>
+        <v>sathiya</v>
       </c>
       <c r="D3" t="str">
-        <v>abc@gmail.com</v>
+        <v>sathiya@gmail.com</v>
       </c>
       <c r="E3" t="str">
-        <v>wipro</v>
+        <v>globalTiger</v>
       </c>
       <c r="F3" t="str">
-        <v>123456791</v>
+        <v>55667788</v>
       </c>
       <c r="G3" t="str">
         <v>offer_rolledout_accepted</v>

</xml_diff>